<commit_message>
Power BI Updates 24092023
</commit_message>
<xml_diff>
--- a/powerbi/powerbi_sample_dataset/district.xlsx
+++ b/powerbi/powerbi_sample_dataset/district.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_39c5\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunilnair/Documents/ByteSize Trainings/curriculum/powerbi/powerbi_sample_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{78FB23F4-DF7C-4428-8B1A-A2C03442591E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7CEB81A-69C8-4862-AB12-A6B9D8183C63}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569902E7-5C13-664D-881F-E5333E147DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="district" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -624,7 +624,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,6 +1159,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{87C78C7E-3FB9-474F-9D1F-3D6FFB11C7F5}" name="district" displayName="district" ref="A1:F78" totalsRowShown="0">
+  <autoFilter ref="A1:F78" xr:uid="{87C78C7E-3FB9-474F-9D1F-3D6FFB11C7F5}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C559C28E-4951-2F45-9D90-1C74D3EFD382}" name="district_code"/>
+    <tableColumn id="2" xr3:uid="{68D35DF1-AC7B-D94D-96E1-BF1F2B9EBE3D}" name="city"/>
+    <tableColumn id="3" xr3:uid="{2CF07DEE-F194-FE40-83A6-CB4981100026}" name="state_name"/>
+    <tableColumn id="4" xr3:uid="{06D83AB4-23FA-D04E-A564-AFC46F8DD9A0}" name="state_abbrev"/>
+    <tableColumn id="5" xr3:uid="{3C22F02E-18B2-6F49-AEB8-8E7D322DD25F}" name="region"/>
+    <tableColumn id="6" xr3:uid="{E1B43DE0-46AC-C540-9B81-11AAE7371FB2}" name="division"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1461,15 +1476,18 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1509,7 +1527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1529,7 +1547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1549,7 +1567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1569,7 +1587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1589,7 +1607,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1609,7 +1627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1629,7 +1647,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1649,7 +1667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1669,7 +1687,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1689,7 +1707,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1709,7 +1727,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1729,7 +1747,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1749,7 +1767,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1769,7 +1787,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1789,7 +1807,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1809,7 +1827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1829,7 +1847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1849,7 +1867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1869,7 +1887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1889,7 +1907,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1909,7 +1927,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1929,7 +1947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1949,7 +1967,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1969,7 +1987,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1989,7 +2007,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2009,7 +2027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2029,7 +2047,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2049,7 +2067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2069,7 +2087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2109,7 +2127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2129,7 +2147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2149,7 +2167,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2169,7 +2187,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2189,7 +2207,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2209,7 +2227,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2229,7 +2247,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2249,7 +2267,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2269,7 +2287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2289,7 +2307,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2309,7 +2327,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2329,7 +2347,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2349,7 +2367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2369,7 +2387,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2389,7 +2407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2409,7 +2427,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2429,7 +2447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2449,7 +2467,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2469,7 +2487,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2489,7 +2507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2509,7 +2527,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2529,7 +2547,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2549,7 +2567,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2569,7 +2587,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2589,7 +2607,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2609,7 +2627,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2629,7 +2647,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2649,7 +2667,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2669,7 +2687,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2689,7 +2707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2709,7 +2727,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2729,7 +2747,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2749,7 +2767,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2769,7 +2787,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2789,7 +2807,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2809,7 +2827,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2829,7 +2847,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2849,7 +2867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2869,7 +2887,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2889,7 +2907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2909,7 +2927,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2929,7 +2947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2949,7 +2967,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2969,7 +2987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2989,7 +3007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3009,7 +3027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3031,5 +3049,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>